<commit_message>
Align WHO Influenza and Mumps with current WHO guidance
- Influenza: convert from universal Standard to Risk series per WHO
  priority groups (pregnant, healthcare workers, immunocompromised,
  chronic conditions, children 6mo-5y, older adults 65+)
- Add observation codes 1023-1026 for influenza risk indications
- Mumps: fix Dose 2 absMinAge 15mo -> 13mo (4 weeks after 12mo dose 1),
  fix earliestRecInt 3mo -> 4 weeks (3mo was MMRV-specific, not MMR),
  remove latestRecAge caps from both doses

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/cicada_generator/lib/WHO/antigen/Influenza.xlsx
+++ b/cicada_generator/lib/WHO/antigen/Influenza.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
     <t xml:space="preserve">Series Name</t>
   </si>
   <si>
-    <t xml:space="preserve">WHO Influenza annual series</t>
+    <t xml:space="preserve">WHO Influenza priority group series</t>
   </si>
   <si>
     <t xml:space="preserve">Target Disease</t>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Series Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard</t>
+    <t xml:space="preserve">Risk</t>
   </si>
   <si>
     <t xml:space="preserve">Equivalent Series Groups</t>
@@ -44,61 +44,109 @@
     <t xml:space="preserve">Select Patient Series</t>
   </si>
   <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO Priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pregnant (1023)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient is pregnant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Healthcare worker (1020)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient is a healthcare worker with occupational exposure risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immunocompromised individual (1022)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient is immunocompromised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chronic medical condition (1024)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient has a chronic medical condition increasing influenza risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO influenza priority - young child (1025)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child aged 6 months to 5 years (WHO priority group)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO influenza priority - older adult (1026)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Older adult aged 65 years or older (WHO priority group)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Series Dose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dose 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferable Vaccine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Influenza, injectable, quadrivalent (150)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowable Vaccine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Influenza, injectable (141)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Influenza, live intranasal (149)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurring Dose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dose 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferable Interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 weeks</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Series Dose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dose 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preferable Vaccine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Influenza, injectable, quadrivalent (150)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allowable Vaccine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Influenza, injectable (141)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Influenza, live intranasal (149)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recurring Dose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dose 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preferable Interval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 weeks</t>
   </si>
 </sst>
 </file>
@@ -407,10 +455,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -435,123 +483,138 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
@@ -560,59 +623,35 @@
         <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
@@ -620,13 +659,13 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -634,24 +673,120 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>